<commit_message>
reporting & Listeners concept
reporting & Listeners concept
</commit_message>
<xml_diff>
--- a/src/test/resources/excelFiles/testdata.xlsx
+++ b/src/test/resources/excelFiles/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Amount</t>
   </si>
@@ -82,19 +82,61 @@
   </si>
   <si>
     <t>thgfvwe23we</t>
+  </si>
+  <si>
+    <t>testCaseDescription</t>
+  </si>
+  <si>
+    <t>ExecutionRequired</t>
+  </si>
+  <si>
+    <t>ListenersClassTest</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>methodName</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>launchBrowser</t>
+  </si>
+  <si>
+    <t>launchportal</t>
+  </si>
+  <si>
+    <t>verifyLogo</t>
+  </si>
+  <si>
+    <t>will launch browser</t>
+  </si>
+  <si>
+    <t>will launch portal</t>
+  </si>
+  <si>
+    <t>will verify logo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -138,10 +180,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -598,12 +642,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>